<commit_message>
add task 0.2 for Iteration 2
</commit_message>
<xml_diff>
--- a/To do List.xlsx
+++ b/To do List.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\Experian\Development\mint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence\GitHub\Mint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13560" windowHeight="6780"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="To do List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do List'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>Item</t>
   </si>
@@ -282,12 +282,21 @@
   <si>
     <t>Bad values in data were preventing auto scale even after Forced Zero was toggled</t>
   </si>
+  <si>
+    <t>Financial Summary</t>
+  </si>
+  <si>
+    <t>Refactor transform qvw to use for..loop to load data extract files of same structures</t>
+  </si>
+  <si>
+    <t>Iteration 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +326,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -338,22 +353,98 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -364,6 +455,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G39" totalsRowCount="1" dataDxfId="10">
+  <autoFilter ref="A1:G38"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Tab" dataDxfId="9"/>
+    <tableColumn id="2" name="Object" dataDxfId="8"/>
+    <tableColumn id="3" name="Item" dataDxfId="7"/>
+    <tableColumn id="4" name="Description" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Notes" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Est Hours" totalsRowFunction="sum" dataDxfId="4"/>
+    <tableColumn id="7" name="Status" dataDxfId="3" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -629,21 +736,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -656,7 +763,7 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -665,648 +772,748 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F2">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
         <v>0.5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F3">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F4">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C6">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="F7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="G7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C7">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
         <v>1.2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C8">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
         <v>1.3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8">
+      <c r="E9" s="4"/>
+      <c r="F9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C9">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
         <v>1.4</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9">
+      <c r="F10" s="3">
         <v>0</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C10">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
         <v>1.5</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C11">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
         <v>1.6</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C12">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
         <v>1.7</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C13">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
         <v>1.8</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F13">
+      <c r="F14" s="3">
         <v>3</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C14">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
         <v>1.9</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F14">
+      <c r="F15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="3">
         <v>2.1</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F15">
+      <c r="F16" s="3">
         <v>0</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F16">
+      <c r="F17" s="3">
         <v>0</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17">
+      <c r="E18" s="4"/>
+      <c r="F18" s="3">
         <v>0</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C18">
+      <c r="C19" s="3">
         <v>2.4</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F18">
+      <c r="F19" s="3">
         <v>0</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="3">
         <v>2.5</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F19">
+      <c r="F20" s="3">
         <v>0</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G20" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C20">
+      <c r="C21" s="3">
         <v>3.1</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F20">
+      <c r="F21" s="3">
         <v>2</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G21" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21">
+      <c r="C22" s="3">
         <v>3.2</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21">
+      <c r="E22" s="4"/>
+      <c r="F22" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C22">
+      <c r="C23" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F22">
+      <c r="F23" s="3">
         <v>0</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C23">
+      <c r="C24" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23">
+      <c r="E24" s="4"/>
+      <c r="F24" s="3">
         <v>0</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G24" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C24">
+      <c r="C25" s="3">
         <v>6.1</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24">
+      <c r="E25" s="4"/>
+      <c r="F25" s="3">
         <v>0</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G25" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C25">
+      <c r="C26" s="3">
         <v>6.2</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F25">
+      <c r="F26" s="3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C26">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
         <v>6.3</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26">
+      <c r="E27" s="4"/>
+      <c r="F27" s="3">
         <v>0</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C27">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
         <v>6.4</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27">
+      <c r="E28" s="4"/>
+      <c r="F28" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C28">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3">
         <v>6.5</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F28">
+      <c r="F29" s="3">
         <v>1</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G29" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C29">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3">
         <v>7.1</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F29">
+      <c r="F30" s="3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C30">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3">
         <v>7.2</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30">
+      <c r="E31" s="4"/>
+      <c r="F31" s="3">
         <v>2</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G31" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C31">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
         <v>7.3</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F31">
+      <c r="F32" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C32">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3">
         <v>7.4</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32">
+      <c r="E33" s="4"/>
+      <c r="F33" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C33">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3">
         <v>8.1</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33">
+      <c r="E34" s="4"/>
+      <c r="F34" s="3">
         <v>0</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G34" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C34">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F34">
+      <c r="F35" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C35">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F35">
+      <c r="F36" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C36">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3">
         <v>8.4</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D39" s="2"/>
+      <c r="E39" s="1"/>
+      <c r="F39">
+        <f>SUBTOTAL(109,Table1[Est Hours])</f>
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push conditional expressions on costs tab, update to do list.
</commit_message>
<xml_diff>
--- a/To do List.xlsx
+++ b/To do List.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13560" windowHeight="6780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="To do List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To do List'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="81">
   <si>
     <t>Item</t>
   </si>
@@ -282,12 +282,24 @@
   <si>
     <t>Bad values in data were preventing auto scale even after Forced Zero was toggled</t>
   </si>
+  <si>
+    <t>Financial Summary</t>
+  </si>
+  <si>
+    <t>Refactor transform qvw to use for..loop to load data extract files of same structures</t>
+  </si>
+  <si>
+    <t>Iteration 2</t>
+  </si>
+  <si>
+    <t>Added conditional expression to trending chart</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +329,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -338,22 +356,98 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -364,6 +458,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G39" totalsRowCount="1" dataDxfId="10">
+  <autoFilter ref="A1:G38"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Tab" dataDxfId="9"/>
+    <tableColumn id="2" name="Object" dataDxfId="8"/>
+    <tableColumn id="3" name="Item" dataDxfId="7"/>
+    <tableColumn id="4" name="Description" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Notes" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Est Hours" totalsRowFunction="sum" dataDxfId="4"/>
+    <tableColumn id="7" name="Status" dataDxfId="3" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -629,21 +739,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -656,7 +766,7 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -665,648 +775,752 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F2">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
         <v>0.5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F3">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F4">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C6">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="F7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="G7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C7">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
         <v>1.2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C8">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
         <v>1.3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8">
+      <c r="E9" s="4"/>
+      <c r="F9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C9">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
         <v>1.4</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9">
+      <c r="F10" s="3">
         <v>0</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C10">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
         <v>1.5</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C11">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
         <v>1.6</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C12">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
         <v>1.7</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C13">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3">
         <v>1.8</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F13">
+      <c r="F14" s="3">
         <v>3</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C14">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3">
         <v>1.9</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F14">
+      <c r="F15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="3">
         <v>2.1</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F15">
+      <c r="F16" s="3">
         <v>0</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F16">
+      <c r="F17" s="3">
         <v>0</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17">
+      <c r="E18" s="4"/>
+      <c r="F18" s="3">
         <v>0</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C18">
+      <c r="C19" s="3">
         <v>2.4</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F18">
+      <c r="F19" s="3">
         <v>0</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="3">
         <v>2.5</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F19">
+      <c r="F20" s="3">
         <v>0</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G20" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C20">
+      <c r="C21" s="3">
         <v>3.1</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F20">
+      <c r="F21" s="3">
         <v>2</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G21" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21">
+      <c r="C22" s="3">
         <v>3.2</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21">
+      <c r="E22" s="4"/>
+      <c r="F22" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C22">
+      <c r="C23" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F22">
+      <c r="F23" s="3">
         <v>0</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G23" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C23">
+      <c r="C24" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23">
+      <c r="E24" s="4"/>
+      <c r="F24" s="3">
         <v>0</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G24" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C24">
+      <c r="C25" s="3">
         <v>6.1</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24">
+      <c r="E25" s="4"/>
+      <c r="F25" s="3">
         <v>0</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G25" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C25">
+      <c r="C26" s="3">
         <v>6.2</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E26" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F25">
+      <c r="F26" s="3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C26">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
         <v>6.3</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26">
+      <c r="E27" s="4"/>
+      <c r="F27" s="3">
         <v>0</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C27">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3">
         <v>6.4</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27">
+      <c r="E28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="G28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C28">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3">
         <v>6.5</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F28">
+      <c r="F29" s="3">
         <v>1</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G29" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C29">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3">
         <v>7.1</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F29">
+      <c r="F30" s="3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C30">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3">
         <v>7.2</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30">
+      <c r="E31" s="4"/>
+      <c r="F31" s="3">
         <v>2</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G31" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C31">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3">
         <v>7.3</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F31">
+      <c r="F32" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C32">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3">
         <v>7.4</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32">
+      <c r="E33" s="4"/>
+      <c r="F33" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C33">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3">
         <v>8.1</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33">
+      <c r="E34" s="4"/>
+      <c r="F34" s="3">
         <v>0</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G34" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C34">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F34">
+      <c r="F35" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C35">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F35">
+      <c r="F36" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C36">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3">
         <v>8.4</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D39" s="2"/>
+      <c r="E39" s="1"/>
+      <c r="F39">
+        <f>SUBTOTAL(109,Table1[Est Hours])</f>
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push to to list
</commit_message>
<xml_diff>
--- a/To do List.xlsx
+++ b/To do List.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="84">
   <si>
     <t>Item</t>
   </si>
@@ -293,6 +293,15 @@
   </si>
   <si>
     <t>Added conditional expression to trending chart</t>
+  </si>
+  <si>
+    <t>Lawrence to rethink UI behavior</t>
+  </si>
+  <si>
+    <t>Low priority</t>
+  </si>
+  <si>
+    <t>Replace the text objects in upper left with "Financial Summary".  Iteration 2</t>
   </si>
 </sst>
 </file>
@@ -742,8 +751,8 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +847,9 @@
       <c r="F4" s="3">
         <v>0.5</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -937,7 +948,9 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -971,9 +984,13 @@
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1003,7 +1020,9 @@
       <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
     </row>
@@ -1061,7 +1080,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
merge with George's status
</commit_message>
<xml_diff>
--- a/To do List.xlsx
+++ b/To do List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\Experian\Development\mint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence\GitHub\Mint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Item</t>
   </si>
@@ -95,32 +95,6 @@
     <t>YTD data changes if a quarter is selected versus not (example: July with Q2 vs. July without selecting Q2)</t>
   </si>
   <si>
-    <r>
-      <t>YTD should always use </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>month</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF222222"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> selected as default; only use Qtr if no month selected.  YTD should always show actuals up through the last month of the Qtr if Qtr selected, not zero (example: through October whether “Oct” selected or “Q3”)</t>
-    </r>
-  </si>
-  <si>
     <t>Dashboard</t>
   </si>
   <si>
@@ -232,9 +206,6 @@
     <t>Need to know what color</t>
   </si>
   <si>
-    <t>Complete Pending Answer</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
@@ -244,12 +215,6 @@
     <t>Ignore any lower grain than year</t>
   </si>
   <si>
-    <t>Pending - will check back with Lori</t>
-  </si>
-  <si>
-    <t>This is on Summary Tab an on ULG Charts.</t>
-  </si>
-  <si>
     <t>Ask Lori more detail on this</t>
   </si>
   <si>
@@ -259,9 +224,6 @@
     <t>Needs Clarification</t>
   </si>
   <si>
-    <t>George</t>
-  </si>
-  <si>
     <t>Bring in new hierarchy qvd provided 3/17</t>
   </si>
   <si>
@@ -271,15 +233,9 @@
     <t>Fix all hardcoded date variables</t>
   </si>
   <si>
-    <t>Development</t>
-  </si>
-  <si>
     <t>Create conditionally shown admin per tab</t>
   </si>
   <si>
-    <t>Complete - Pending review</t>
-  </si>
-  <si>
     <t>Bad values in data were preventing auto scale even after Forced Zero was toggled</t>
   </si>
   <si>
@@ -289,17 +245,65 @@
     <t>Refactor transform qvw to use for..loop to load data extract files of same structures</t>
   </si>
   <si>
-    <t>Iteration 2</t>
-  </si>
-  <si>
     <t>Added conditional expression to trending chart</t>
+  </si>
+  <si>
+    <t>Codebase</t>
+  </si>
+  <si>
+    <t>Load script</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Lawrence to rethink UI behavior</t>
+  </si>
+  <si>
+    <t>depends on Item 0.5</t>
+  </si>
+  <si>
+    <t>Low priority</t>
+  </si>
+  <si>
+    <t>Replace the text objects in upper left with "Financial Summary".  Iteration 2</t>
+  </si>
+  <si>
+    <t>YTD should always use month selected as default; only use Qtr if no month selected.  YTD should always show actuals up through the last month of the Qtr if Qtr selected, not zero (example: through October whether “Oct” selected or “Q3”)</t>
+  </si>
+  <si>
+    <t>Complete - Pending Review</t>
+  </si>
+  <si>
+    <t>Complete - Pending Answer</t>
+  </si>
+  <si>
+    <t>Rename the tab to Trends</t>
+  </si>
+  <si>
+    <t>Lori and Bob to discuss and decide how if the sign to be flipped on the ULG chart (vs. on the P&amp;L and the Financial Summary)</t>
+  </si>
+  <si>
+    <t>This is on Summary Tab and on ULG Charts.</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Iteration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,14 +319,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
@@ -361,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,14 +372,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -407,6 +403,9 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -461,16 +460,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G39" totalsRowCount="1" dataDxfId="10">
-  <autoFilter ref="A1:G38"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Tab" dataDxfId="9"/>
-    <tableColumn id="2" name="Object" dataDxfId="8"/>
-    <tableColumn id="3" name="Item" dataDxfId="7"/>
-    <tableColumn id="4" name="Description" dataDxfId="6" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="Notes" dataDxfId="5" totalsRowDxfId="1"/>
-    <tableColumn id="6" name="Est Hours" totalsRowFunction="sum" dataDxfId="4"/>
-    <tableColumn id="7" name="Status" dataDxfId="3" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H39" totalsRowCount="1" dataDxfId="11">
+  <autoFilter ref="A1:H38"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Tab" dataDxfId="10"/>
+    <tableColumn id="2" name="Object" dataDxfId="9"/>
+    <tableColumn id="3" name="Item" dataDxfId="8"/>
+    <tableColumn id="4" name="Description" dataDxfId="7" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Notes" dataDxfId="6" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Est Hours" totalsRowFunction="sum" dataDxfId="5"/>
+    <tableColumn id="7" name="Status" dataDxfId="4" totalsRowDxfId="0"/>
+    <tableColumn id="8" name="Iteration" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -739,11 +739,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,14 +754,15 @@
     <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -778,19 +779,22 @@
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="3">
         <v>0.1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3">
@@ -799,19 +803,22 @@
       <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="3">
         <v>0.2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3">
@@ -820,69 +827,85 @@
       <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3">
         <v>0.3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3">
         <v>0.5</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3">
         <v>0.4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C6" s="3">
         <v>0.5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>79</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3">
-        <v>2</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3">
@@ -900,10 +923,13 @@
       <c r="G7" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3">
@@ -921,10 +947,13 @@
       <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3">
@@ -937,11 +966,16 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -959,10 +993,13 @@
       <c r="G10" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
@@ -971,13 +1008,22 @@
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
@@ -986,15 +1032,22 @@
       <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
       <c r="G12" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
@@ -1003,13 +1056,22 @@
       <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3">
@@ -1025,12 +1087,15 @@
         <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3">
@@ -1045,14 +1110,19 @@
       <c r="F15" s="3">
         <v>0</v>
       </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="G15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="3">
         <v>2.1</v>
@@ -1061,21 +1131,24 @@
         <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="F16" s="3">
         <v>0</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3">
         <v>2.2000000000000002</v>
@@ -1084,159 +1157,182 @@
         <v>21</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="F17" s="3">
         <v>0</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3">
         <v>2.2999999999999998</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="3">
         <v>0</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="3">
         <v>2.4</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" s="3">
         <v>0</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3">
         <v>2.5</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="F20" s="3">
         <v>0</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3">
         <v>3.1</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F21" s="3">
         <v>2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="3">
         <v>3.2</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3">
         <v>3</v>
       </c>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="3">
         <v>0</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="3">
         <v>5.0999999999999996</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3">
@@ -1245,59 +1341,72 @@
       <c r="G24" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C25" s="3">
         <v>6.1</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="F25" s="3">
         <v>0</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C26" s="3">
         <v>6.2</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F26" s="3">
         <v>1.5</v>
       </c>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
         <v>6.3</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="3">
@@ -1306,20 +1415,23 @@
       <c r="G27" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3">
         <v>6.4</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F28" s="3">
         <v>4</v>
@@ -1327,20 +1439,23 @@
       <c r="G28" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3">
         <v>6.5</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
@@ -1348,91 +1463,114 @@
       <c r="G29" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3">
         <v>7.1</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F30" s="3">
         <v>1.5</v>
       </c>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3">
         <v>7.2</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="F31" s="3">
         <v>2</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3">
         <v>7.3</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="F32" s="3">
         <v>4</v>
       </c>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3">
         <v>7.4</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="3">
         <v>2</v>
       </c>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G33" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3">
         <v>8.1</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="3">
@@ -1441,79 +1579,110 @@
       <c r="G34" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3">
         <v>8.1999999999999993</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F35" s="3">
         <v>4</v>
       </c>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="G35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H35" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3">
         <v>8.3000000000000007</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F36" s="3">
         <v>4</v>
       </c>
-      <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G36" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H36" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3">
         <v>8.4</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="3">
+        <v>18</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39" s="2"/>
       <c r="E39" s="1"/>
       <c r="F39">
         <f>SUBTOTAL(109,Table1[Est Hours])</f>
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>